<commit_message>
add emnlp best paper data
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -821,6 +821,31 @@
   <si>
     <t>Database
 API-call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiWOZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMNLP 2018 best paper, not release yet.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paper:
+MultiWOZ - A Large-Scale Multi-Domain Wizard-of-Oz Dataset for Task-Oriented Dialogue Modelling（Not Released Yet）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1194,9 +1219,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G14" sqref="G14"/>
     </sheetView>
@@ -1568,6 +1593,38 @@
         <v>96</v>
       </c>
     </row>
+    <row r="12" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add 6 new datasets
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,10 +43,6 @@
   </si>
   <si>
     <t>Included Label</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Missing Label</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -123,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>灵犀数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Task Oriented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -649,10 +641,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Stanford Dialog Dataset Labeled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dialogue level database
 User Act(inform, request slots)
 Agent Act(inform, request slots)</t>
@@ -714,38 +702,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Stanford data labeled by us, relabel slot &amp; intent
-2. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Human2Human</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3. A quick intro http://m.sohu.com/n/499803391/ to stanford data
-4. Annotation handbook: https://docs.google.com/document/d/1ROARKf8AJNnG2_nPINe1Xm5Rza7V0jPnQV8io09hcFY/edit</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Booking  restautant </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -769,41 +725,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">human-annotated conversational data in three domains (movie-ticket booking, restaurant reservation, and taxi booking), 
-as well as an experiment platform </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>with built-in simulators</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in each domain, for training and evaluation purposes. </t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -814,38 +736,542 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Database
+API-call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiWOZ 2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Oriented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Oriented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Proposed by EMNLP 2018 best paper.
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Largest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by now &amp; contain </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">multi-domains.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Human2human
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> goal changes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>are encouraged</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 domains
+Attraction, Hospital,
+Police, Hotel, Restaurant, Taxi, Train.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Download:
+http://dialogue.mi.eng.cam.ac.uk/index.php/corpus/
+Paper:
+https://arxiv.org/pdf/1810.00278.pdf
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Belief state
+User Act(inform, request slots)
+Agent Act(inform, request slots)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLU(Intent, Slots)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snips</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+https://github.com/snipsco/
+nlu-benchmark/tree/master/ 2017-06-custom-intent-engines</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total 10438 dialogues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+average number of turns are 8.93 and 15.39 for single and multi-domain dialogues respectively.
+115, 434 turns in total.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train:13,084 
+Test:700
+7 intent 72 slot labels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Intent
 Slots</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Database
-API-call</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MultiWOZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EMNLP 2018 best paper, not release yet.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Paper:
-MultiWOZ - A Large-Scale Multi-Domain Wizard-of-Oz Dataset for Task-Oriented Dialogue Modelling（Not Released Yet）</t>
+    <t>ATIS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The ATIS (Airline Travel Information Systems) dataset (Tur et al., 2010) is widely used in SLU research
+2.  For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>natural language understanding</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Oriented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Airline Travel Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train: 4478
+Test: 893
+120 slot and 21 intent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent
+Slots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent
+Slots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+1. https://github.com/AtmaHou/Bi-LSTM_PosTagger/tree/master/data
+2.https://github.com/yvchen/JointSLU/tree/master/data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Containing human-annotated conversational data in three domains  an 
+2. Experiment platform </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with built-in simulators</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in each domain, for training and evaluation purposes. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medical DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Download:
+http://www.sdspeople.fudan.edu.cn/zywei/data/acl2018-mds.zip
+Paper: 
+http://www.sdspeople.fudan.edu.cn/zywei/paper/liu-acl2018.pdf
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. Our dataset is collected from the pediatric department in a Chinese online healthcare community
+2. Task-oriented Dialogue System for</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Automatic Diagnosis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatic Diagnosis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 Disease
+67 symptoms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot
+Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT Restaurant Corpus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Collected by Snips for model evaluation.
+2. For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>natural language understanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Homepage: https://medium.com/snips-ai/benchmarking-natural-language-understanding-systems-google-facebook-microsoft-and-snips-2b8ddcf9fb19</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT Movie Corpus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The MIT Restaurant Corpus is a semantically tagged training and test corpus in BIO format.
+2.  For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>natural language understanding</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The MIT Movie Corpus is a semantically tagged training and test corpus in BIO format. The eng corpus are simple queries, and the trivia10k13 corpus are more complex queries.
+2. For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>natural language understanding</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+https://groups.csail.mit.edu/sls/downloads/restaurant/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+https://groups.csail.mit.edu/sls/downloads/movie/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 task:
+Weather,play music, search, add to list, book, moive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resaurant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train, Dev, Test
+6,894 766 1,521</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train, Dev, Test
+MIT Movie Eng 8,798 977 2,443
+MIT Movie Trivia 7,035 781 1,953
+Refer to: Data Augmentation for Spoken Language Understanding via Joint Variational Generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lingxi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stanford Dialog Dataset LU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Stanford data labeled by HIT, relabel slot &amp; intent
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Human2Human</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. A quick intro http://m.sohu.com/n/499803391/ to stanford data
+4. Annotation handbook: https://docs.google.com/document/d/1ROARKf8AJNnG2_nPINe1Xm5Rza7V0jPnQV8io09hcFY/edit</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missing Label</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1219,22 +1645,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="49.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.875" style="1" customWidth="1"/>
@@ -1249,380 +1675,531 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="114" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>80</v>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>84</v>
+    <row r="15" spans="1:10" ht="114" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="16" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="J17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="114" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="57" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add TOP semantic parsing dataset
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Research\TaskOrientedDialogue\Resource\SurveyAndNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sz128/workspace/data/Task-Oriented-Dialogue-Dataset-Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A338A63E-97E4-C441-B7A7-3D66B8F883AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="5010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,10 +175,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Booking  restautant </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://camdial.org/~mh521/dstc/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -538,10 +535,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Querry touristic information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,10 +695,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Booking  restautant </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Microsoft Dialogue Challenge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1191,14 +1180,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Resaurant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Movive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1274,12 +1255,123 @@
     <t>Missing Label</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>TOP semantic parsing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+http://fb.me/semanticparsingdialog
+Paper: 
+https://arxiv.org/pdf/1810.07942.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task Oriented</t>
+  </si>
+  <si>
+    <t>Hierarchical intents
+Slots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train 31279 utterances
+Dev 4462 utterances
+Test 9042 utterances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Movie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restaurant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking  restaurant </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query touristic information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Navigation and event</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. (Facebook) A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hierarchical</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> semantic representation for task oriented dialog systems that can model compositional and nested queries. (hierarchical intent and slot)
+2. For </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>natural language understanding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Human2bot</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1326,6 +1418,15 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1644,30 +1745,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="49.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="2"/>
+    <col min="9" max="9" width="28.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,303 +1788,303 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="96">
       <c r="A2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="112">
+      <c r="A3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="64">
+      <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="48">
       <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="80">
       <c r="A6" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="80">
       <c r="A7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>114</v>
-      </c>
     </row>
-    <row r="8" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="64">
       <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>89</v>
-      </c>
     </row>
-    <row r="9" spans="1:10" ht="134.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="134.5" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="147" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="144">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -2007,15 +2108,15 @@
         <v>18</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="112">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -2036,21 +2137,21 @@
         <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="114" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="128">
       <c r="A13" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>28</v>
@@ -2062,27 +2163,27 @@
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="86.5" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
@@ -2091,62 +2192,62 @@
         <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="114" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="96">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="64">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="57" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>28</v>
@@ -2155,24 +2256,24 @@
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="17" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="84" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>24</v>
@@ -2184,7 +2285,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
@@ -2199,9 +2300,39 @@
         <v>23</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
+    <row r="18" spans="1:10" ht="90" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Facebook Multilingual Task Oriented Dataset
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sz128/workspace/data/Task-Oriented-Dialogue-Dataset-Survey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kronej/Developer/Task-Oriented-Dialogue-Dataset-Survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A338A63E-97E4-C441-B7A7-3D66B8F883AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0CCD7B-904A-E04B-88F9-E5DABEC9AB5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14440" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,7 +228,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -239,7 +239,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -260,7 +260,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -271,7 +271,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -292,7 +292,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -303,7 +303,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -323,7 +323,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -334,7 +334,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -387,7 +387,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -435,7 +435,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -446,7 +446,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -459,7 +459,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -495,7 +495,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -508,7 +508,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -521,7 +521,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -561,7 +561,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -580,7 +580,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -591,7 +591,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -670,7 +670,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -681,7 +681,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -755,7 +755,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -766,7 +766,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -778,7 +778,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -790,7 +790,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -802,7 +802,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -814,7 +814,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -826,7 +826,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -837,7 +837,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -898,7 +898,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -909,7 +909,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -945,7 +945,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -998,7 +998,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1009,7 +1009,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1044,7 +1044,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1055,7 +1055,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1097,7 +1097,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1108,7 +1108,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1132,7 +1132,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1151,7 +1151,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1229,7 +1229,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1240,7 +1240,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1309,7 +1309,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1320,7 +1320,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1333,7 +1333,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1344,7 +1344,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1357,7 +1357,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1365,24 +1365,62 @@
       <t>Human2bot</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facebook Multilingual Task Oriented Dataset</t>
+  </si>
+  <si>
+    <t>English Train: 30,521
+English Dev: 4,181
+English Test: 8,621
+Spanish Train: 3,617
+Spanish Dev: 1,983
+Spanish Test: 3,043
+Thai Train: 2,156
+Thai Dev: 1,235
+Thai Test:  1,692</t>
+  </si>
+  <si>
+    <t>Slot
+Intent</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>3 Domains: Alarm, Reminder, Weather
+3 Languages: English, Spanish, Thai</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>1. (Faceboook)  We release a dataset of around 57k annotated utterances
+in English (43k), Spanish (8.6k) and Thai (5k) for three task oriented domains … ALARM,
+REMINDER, and WEATHER.
+2. For cross-lingual natural language understanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download: https://fb.me/multilingual_task_oriented_data 
+Paper: https://arxiv.org/pdf/1810.13327.pdf </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1390,7 +1428,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1398,7 +1436,7 @@
     <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1407,7 +1445,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1416,7 +1454,7 @@
       <b/>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1425,7 +1463,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1468,7 +1506,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1748,12 +1786,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
@@ -1768,7 +1806,7 @@
     <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1800,7 +1838,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96">
+    <row r="2" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -1832,7 +1870,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="112">
+    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
@@ -1861,7 +1899,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="64">
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -1890,7 +1928,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="48">
+    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -1922,7 +1960,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="80">
+    <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
@@ -1954,7 +1992,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80">
+    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>104</v>
       </c>
@@ -1983,7 +2021,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="64">
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>80</v>
       </c>
@@ -2015,7 +2053,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="134.5" customHeight="1">
+    <row r="9" spans="1:10" ht="134.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2047,7 +2085,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="147" customHeight="1">
+    <row r="10" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -2079,7 +2117,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="144">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2111,7 +2149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="112">
+    <row r="12" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2181,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="128">
+    <row r="13" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>139</v>
       </c>
@@ -2175,7 +2213,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="86.5" customHeight="1">
+    <row r="14" spans="1:10" ht="86.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -2207,7 +2245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="96">
+    <row r="15" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -2239,7 +2277,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="64">
+    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2271,7 +2309,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="84" customHeight="1">
+    <row r="17" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>138</v>
       </c>
@@ -2303,7 +2341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="90" customHeight="1">
+    <row r="18" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>142</v>
       </c>
@@ -2332,7 +2370,35 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16" customHeight="1"/>
+    <row r="19" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 10 dataset, 5 results, 1 correctness
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kronej/Developer/Task-Oriented-Dialogue-Dataset-Survey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Project\Web\Task-Oriented-Dialogue-Dataset-Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0CCD7B-904A-E04B-88F9-E5DABEC9AB5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A70B0D-01D0-4D09-894C-3E5C955F419E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14440" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14436" yWindow="0" windowWidth="14364" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="223">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,15 +39,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Included Label</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task Oriented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -83,10 +75,6 @@
   </si>
   <si>
     <t>Book a table at a restaurant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task Oriented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -120,10 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>conversational robot service user log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,10 +189,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,7 +208,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -239,7 +219,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -260,7 +240,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -271,7 +251,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -292,7 +272,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -303,7 +283,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -323,7 +303,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -334,7 +314,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -360,10 +340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Travel Booking</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -387,7 +363,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -435,7 +411,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -446,7 +422,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -459,7 +435,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -495,7 +471,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -508,7 +484,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -521,7 +497,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -561,7 +537,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -580,7 +556,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -591,7 +567,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -670,7 +646,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -681,7 +657,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -738,14 +714,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task Oriented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">1. Proposed by EMNLP 2018 best paper.
 2. </t>
@@ -755,7 +723,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -766,7 +734,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -778,7 +746,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -790,7 +758,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -802,7 +770,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -814,7 +782,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -826,7 +794,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -837,7 +805,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -898,7 +866,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -909,7 +877,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -945,17 +913,13 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>natural language understanding</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Task Oriented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -998,7 +962,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1009,7 +973,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1044,7 +1008,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1055,7 +1019,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1097,7 +1061,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1108,7 +1072,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1132,7 +1096,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1151,7 +1115,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1229,7 +1193,7 @@
         <b/>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1240,7 +1204,7 @@
       <rPr>
         <sz val="10.5"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1267,9 +1231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Task Oriented</t>
-  </si>
-  <si>
     <t>Hierarchical intents
 Slots</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1309,7 +1270,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1320,7 +1281,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1333,7 +1294,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1344,7 +1305,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1357,7 +1318,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1404,23 +1365,570 @@
     <t xml:space="preserve">Download: https://fb.me/multilingual_task_oriented_data 
 Paper: https://arxiv.org/pdf/1810.13327.pdf </t>
   </si>
+  <si>
+    <t>Schema-Guided Dialogue State Tracking(DST8)</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>16 domains Alarm, Banks, Buses, Calendar, Events, Flights, Homes, Media, Messaging, Movies, etc.</t>
+  </si>
+  <si>
+    <t>Over 16k dialogues average number of turns are 20.44 multi-domain dialogues. 329,964 turns in total.</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>Schema for each service contains: 
+service_name and description, 
+slots, 
+intents</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Download: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://github.com/google-research-datasets/dstc8-schema-guided-dialogue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> 
+Paper: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0366D6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://arxiv.org/pdf/1909.05855.pdf</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minecraft Dialogue corpus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: http://juliahmr.cs.illinois.edu/Minecraft/
+Paper: https://www.aclweb.org/anthology/P19-1537.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. Largest by now &amp; containing over 16k multi-domain conversations spanning </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>16 domains</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> 
+2. Present a schema-guided paradigm 
+3. Enable zero-shot generalization to new APIs</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Architect" instruct the "Builder" to build a 3D structure.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>509 human-human dialogues;
+15,926 utterances (train 6,548,  dev 2,855, test 2,251 Architect utterances);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. The goal of this project is to develop systems that can collaborate and communicate with each other to solve tasks in a 3D environment.
+2.  Human2Human
+3.  Main task: given context and 3D scenes, generating response.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 dialogue task:
+Weather,play music, search, add to list, book, moive
+5 NER task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For each task, it contains 100 episodes. 
+Each episode contains a query set (20 samples) and a support set (1-shot &amp; 5-shot)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Few-shot Slot Tagging Benchmark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Dialogue slot tagging dataset for few-shot learning setting
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First few-shot sequence labeling benchmark</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Meta-episode style data format)
+3. Also include 5  NER dataset for few-shot sequence labeling evaluation.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:https://atmahou.github.io/attachments/ACL2020data.zip
+Paper: https://arxiv.org/pdf/2006.05702.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://www.microsoft.com/en-us/download/58389
+Homepage: https://www.microsoft.com/en-us/research/project/metalwoz/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Dialogue dataset for developing fast adaptation methods for conversation models. (Track in DSTC 8)
+2. Lots of domains and tasks: 47 domains and 227 tasks. 
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Suitable for meta learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+4. Main task: dialogue generation</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>37,884</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">dialogues, ( &gt;10 turns long),
+47 domains and 227 tasks. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">47 domains and 227 tasks. </t>
+  </si>
+  <si>
+    <t>Only utterance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multimodal Dialogs (MMD) Dataset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shopping Assistant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150K conversation session</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>question-type (Intent)
+State Type (17 type of dialogue state class)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaLWOz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multimodal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> conversations in the fashion domain. 
+2. Human-to-human
+3. Contain annotation of query type (Similar to intent)
+4. Large size: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>150K conversation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: http://jddc.jd.com/auth_environment
+Paper: https://arxiv.org/pdf/1911.09969.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> E-commerce conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  A large-scale real scenario Chinese E-commerce conversation corpus.
+2.   Human-human conversations covers: task-oriented, chitchat and question-answering.
+3. Large scale: 1 million multi-turn dialogues, 20 million utterances.
+4. Main task: dialogue generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent, 
+Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JDDC Corpus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Dialogue utterances from the Chinese Artificial Intelligence Speakers (CAIS) annotated with slot tags and intent labels.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://amritasaha1812.github.io/MMD/ 
+Paper:
+https://arxiv.org/abs/1704.00200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://github.com/Adaxry/CM-Net 
+Paper: https://www.aclweb.org/anthology/D19-1097.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Most are music related tasks.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train 7995;
+Dev 994;
+Test 1012;
+11 Intents, 75 Slots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API calls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taskmaster-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://g.co/dataset/taskmaster-1
+Paper: https://arxiv.org/pdf/1909.05358.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 domains: ordering pizza, creating auto repair appointments, setting up ride service, ordering movie tickets, ordering coffee drinks and making restaurant reservations.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Human-Human: 7,708 dialogues, 169,469 utterances
+Human-Machine: 10,438 dialogues, 132,610 utterances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API calls,
+Argument (Slot)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. A task-based dataset collect with two different procedures: Wizard of Oz and self conversation.
+2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Encourage realistic and diversity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by giving up restrict speaker with knowledage base.
+3. Both Human2machine and Human2Human dialogues</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. The Switchboard Dialog Act Corpus (SwDA) extends the Switchboard-1 Telephone Speech Corpus, Release 2, with turn/utterance-level dialog-act tags.
+2. The tags summarize syntactic, semantic, and pragmatic information about the associated turn. The SwDA project was undertaken at UC Boulder in the late 1990s.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAIS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switchboard Dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: http://compprag.christopherpotts.net/swda.html
+Instruction: https://web.stanford.edu/~jurafsky/ws97/manual.august1.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train: 197,489 training-set utterances, 1115 conversations
+Test: 40 conversations
+Annotation: 42 Classes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CrossWOZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://github.com/thu-coai/CrossWOZ 
+Paper: https://arxiv.org/pdf/2002.11893.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 domains, including hotel, restaurant, attraction, metro, and taxi.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. CrossWOZ, the first large-scale Chinese Cross-Domain Wizard-of-Oz taskoriented dataset.
+2. Encourage natural transition across domains in conversation.
+3. Provide a user simulator 
+4. Human2Human</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Totoal: 1 million dialogues, 20 million utterances.
+Annotation: 289 different intents
+Challenge1: 300 dialogues,  300 questions;
+Challenge2: 15 dialogues,  168 questions;
+Challenge3: 108 dialogues,  500 questions;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,012 dialogues,
+84,692 turns,
+16.9 Avg. turns,
+Annotation:
+72 slots, 7,871 vlaues, 6 intents</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Goals,
+State (Intent, Slots),
+Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-commerce Dialogue Corpus (EDC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:
+https://github.com/cooelf/ 
+Paper: https://arxiv.org/pdf/1806.09102.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  Real-world conversations between customers and
+customer service staff from our E-commerce partners in Taobao
+2.  Main task: response selection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contains 5 types of conversations: commodity consultation, logistics express, recommendation, negotiation and chitchat based on over 20 commodities.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialogues 1,020,000, 
+Utterance 7,500,000.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Golden utterance,
+game log,
+screenshots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1428,7 +1936,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1436,7 +1944,7 @@
     <font>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1445,7 +1953,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1454,7 +1962,7 @@
       <b/>
       <sz val="10.5"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1463,26 +1971,71 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0366D6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF505050"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1491,7 +2044,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1504,9 +2057,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1784,619 +2352,877 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="49.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.83203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="2"/>
+    <col min="3" max="3" width="37.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="169.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="134.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="86.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="134.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="86.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>155</v>
+    <row r="30" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 3 dataset, 3 results re-claim; refine layout
</commit_message>
<xml_diff>
--- a/Atma'sDatasetSurvey.xlsx
+++ b/Atma'sDatasetSurvey.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Project\Web\Task-Oriented-Dialogue-Dataset-Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A70B0D-01D0-4D09-894C-3E5C955F419E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24438115-7E66-46CE-8C4F-DAEA7BFC3F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14436" yWindow="0" windowWidth="14364" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="236">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1703,23 +1703,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.  A large-scale real scenario Chinese E-commerce conversation corpus.
-2.   Human-human conversations covers: task-oriented, chitchat and question-answering.
-3. Large scale: 1 million multi-turn dialogues, 20 million utterances.
-4. Main task: dialogue generation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Slot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intent, 
-Database</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JDDC Corpus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1750,10 +1734,6 @@
   </si>
   <si>
     <t>API calls</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taskmaster-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1912,12 +1892,149 @@
 screenshots</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>JDDC Corpus 2019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JDDC Corpus 2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.  A large-scale real scenario Chinese E-commerce conversation corpus.
+2.  Human2Human conversations covers: task-oriented, chitchat and question-answering.
+3. Large scale: 1 million multi-turn dialogues, 20 million utterances.
+4. Main task: dialogue generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. A large-scale </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multimodal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Chinese E-commerce conversation corpus.
+2. Human2Human conversations</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download:  https://jddc.jd.com/auth_environment
+Homepage: https://jddc.jd.com/description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Multimodal E-commerce conversation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electronic: 130k dialogues, 950k utterances, 215k images.
+Clothing:  116k dialogues, 810k utterances, 200k images.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intent (Machine Labeled), 
+Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intents (Only on images),
+Database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taskmaster-1 (2019)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taskmaster-2 (2020)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. Unlike Taskmaster-1, which includes both written "self-dialogs" and spoken two-person dialogs, Taskmaster-2 consists entirely of spoken two-person dialogs.
+2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Users were led to believe they were interacting with an automated system that “spoke” using text-to-speech (TTS)
+3. Intents are labeled on slots</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download: https://github.com/google-research-datasets/Taskmaster/tree/master/TM-2-2020/data
+Homepage: https://github.com/google-research-datasets/Taskmaster/tree/master/TM-2-2020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,289 dialogs:
+restaurants (3276)
+food ordering (1050)
+movies (3047)
+hotels (2355)
+flights (2481)
+music (1602)
+sports (3478)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 domains:
+restaurants, food ordering, movies, hotels, flights, music, sports</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1975,12 +2092,6 @@
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF24292E"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2066,7 +2177,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2352,11 +2463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2431,227 +2542,224 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>163</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>95</v>
+        <v>212</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>179</v>
+    <row r="6" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>219</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>163</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>197</v>
+      <c r="A7" t="s">
+        <v>201</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>163</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>183</v>
+      <c r="A8" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>176</v>
+      <c r="G8" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>163</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>217</v>
+    <row r="10" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>221</v>
+      <c r="G10" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>178</v>
@@ -2660,569 +2768,627 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>155</v>
+    <row r="11" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>214</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>85</v>
+        <v>163</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>217</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="169.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:9" ht="75.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="169.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="69" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:9" ht="69" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="134.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:9" ht="134.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:9" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" ht="124.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="124.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="26" spans="1:9" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="86.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="27" spans="1:9" ht="86.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>25</v>
+      <c r="D28" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>141</v>
+        <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>188</v>
+      <c r="H32" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>